<commit_message>
drop duplicates was added, the key column composition was added to the configuration
</commit_message>
<xml_diff>
--- a/configs/attributes_notification.xlsx
+++ b/configs/attributes_notification.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demid\Documents\ИНК\python_ink\appius-mto-neosintez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demid\Documents\python\work_projects\appius-mto-neosintez\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6A6869-1EB5-4D41-9A00-EE49680A3F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E5BEEC-2FC4-4904-8C7B-AFA957034671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -135,10 +135,16 @@
     <t>cb67f5e8-0315-ea11-910b-005056b6948b</t>
   </si>
   <si>
-    <t>Потребность-Дата отгрузки-Дата прихода</t>
-  </si>
-  <si>
     <t>Резервирование/Планирование закупок/Спецификация/РасходныйДокумент/Поступление/Уведомление об отгрузке.Договор.Контрагент, Код</t>
+  </si>
+  <si>
+    <t>Потребность-Уведомление</t>
+  </si>
+  <si>
+    <t>6532ec8d-56cd-ed11-9165-005056b6948b</t>
+  </si>
+  <si>
+    <t>Резервирование/Планирование закупок/Спецификация/РасходныйДокумент/Поступление/Уведомление об отгрузке.Номер</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный_Лист3" xfId="1" xr:uid="{CC9F1E92-83C7-4075-9C41-317146FF9CBC}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -211,9 +217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -251,7 +257,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -357,7 +363,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,7 +516,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -688,7 +694,18 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">

</xml_diff>